<commit_message>
2nd round of results for Iris
</commit_message>
<xml_diff>
--- a/Outputs/Iris_mean_results.xlsx
+++ b/Outputs/Iris_mean_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giparoli\Documents\Projetos\AEco\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FFA838-C2BC-43FF-8149-F96CF9ABFA3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488DE89B-4270-43D4-AE50-CA6C0DC3772D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="absolute" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,20 @@
     <sheet name="absolute - EP" sheetId="3" r:id="rId3"/>
     <sheet name="relative - EP" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
   <si>
     <t>Categories</t>
   </si>
@@ -110,17 +118,24 @@
   </si>
   <si>
     <t>RA</t>
+  </si>
+  <si>
+    <t>at x updt</t>
+  </si>
+  <si>
+    <t>og x updt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +153,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -147,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -185,11 +207,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -202,9 +236,15 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -504,15 +544,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G19"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -535,7 +580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -557,8 +602,20 @@
       <c r="G2" s="4">
         <v>2.4351909812311529E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="9">
+        <f>(E2-C2)/C2</f>
+        <v>-0.2502952718465441</v>
+      </c>
+      <c r="I2" s="7">
+        <f>G2-E2</f>
+        <v>3.0281016079815072E-3</v>
+      </c>
+      <c r="J2" s="8">
+        <f>I2/G2</f>
+        <v>0.12434760276791917</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -580,8 +637,20 @@
       <c r="G3" s="4">
         <v>0.57921014222493539</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="9">
+        <f t="shared" ref="H3:H19" si="0">(E3-C3)/C3</f>
+        <v>-0.17678881959978093</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="shared" ref="I3:I19" si="1">G3-E3</f>
+        <v>4.0036852958468483E-2</v>
+      </c>
+      <c r="J3" s="8">
+        <f t="shared" ref="J3:J19" si="2">I3/G3</f>
+        <v>6.9123190427353098E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -603,8 +672,20 @@
       <c r="G4" s="4">
         <v>26.413936343283179</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.25050970695243635</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="1"/>
+        <v>3.2839474999596696</v>
+      </c>
+      <c r="J4" s="8">
+        <f t="shared" si="2"/>
+        <v>0.12432631991235744</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -626,8 +707,20 @@
       <c r="G5" s="4">
         <v>38.263494119156263</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.25037515302451824</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="1"/>
+        <v>4.7526574062286642</v>
+      </c>
+      <c r="J5" s="8">
+        <f t="shared" si="2"/>
+        <v>0.12420866195409191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -649,8 +742,20 @@
       <c r="G6" s="4">
         <v>0.3410444655401067</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.24931957565227197</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="1"/>
+        <v>4.2618102465567076E-2</v>
+      </c>
+      <c r="J6" s="8">
+        <f t="shared" si="2"/>
+        <v>0.12496347770392187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -672,8 +777,20 @@
       <c r="G7" s="4">
         <v>8.118861636150406</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.25050079322230617</v>
+      </c>
+      <c r="I7" s="7">
+        <f t="shared" si="1"/>
+        <v>1.0093694058399336</v>
+      </c>
+      <c r="J7" s="8">
+        <f t="shared" si="2"/>
+        <v>0.1243240063786246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -695,8 +812,20 @@
       <c r="G8" s="4">
         <v>0.1039077908990419</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.24906323254440244</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" si="1"/>
+        <v>1.2994500517184079E-2</v>
+      </c>
+      <c r="J8" s="8">
+        <f t="shared" si="2"/>
+        <v>0.12505800002821441</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -718,8 +847,20 @@
       <c r="G9" s="4">
         <v>414.14533902212662</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.25052181677785679</v>
+      </c>
+      <c r="I9" s="7">
+        <f t="shared" si="1"/>
+        <v>51.481913338272534</v>
+      </c>
+      <c r="J9" s="8">
+        <f t="shared" si="2"/>
+        <v>0.12430880777224441</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -741,8 +882,20 @@
       <c r="G10" s="4">
         <v>207.20104990685169</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.25050641889707959</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="1"/>
+        <v>25.755091921422803</v>
+      </c>
+      <c r="J10" s="8">
+        <f t="shared" si="2"/>
+        <v>0.12430000684360015</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -764,8 +917,20 @@
       <c r="G11" s="4">
         <v>1.326597815114525E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.24910851060695544</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="1"/>
+        <v>1.6454315073734108E-4</v>
+      </c>
+      <c r="J11" s="8">
+        <f t="shared" si="2"/>
+        <v>0.12403393768829334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -787,8 +952,20 @@
       <c r="G12" s="4">
         <v>6.1572623439631637E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.25043357701203284</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="1"/>
+        <v>7.649757612033084E-3</v>
+      </c>
+      <c r="J12" s="8">
+        <f t="shared" si="2"/>
+        <v>0.12423959195978103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -810,8 +987,20 @@
       <c r="G13" s="4">
         <v>2.163426205441121E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.24956558438125589</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="1"/>
+        <v>2.6973170683931985E-3</v>
+      </c>
+      <c r="J13" s="8">
+        <f t="shared" si="2"/>
+        <v>0.12467802514406622</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -833,8 +1022,20 @@
       <c r="G14" s="4">
         <v>3.239303265867802</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.2497137426380758</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.40287550014266182</v>
+      </c>
+      <c r="J14" s="8">
+        <f t="shared" si="2"/>
+        <v>0.12437103508884723</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -856,8 +1057,20 @@
       <c r="G15" s="4">
         <v>319423.80450478522</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.2503032715132541</v>
+      </c>
+      <c r="I15" s="7">
+        <f t="shared" si="1"/>
+        <v>39651.874803785817</v>
+      </c>
+      <c r="J15" s="8">
+        <f t="shared" si="2"/>
+        <v>0.1241356287308005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -879,8 +1092,20 @@
       <c r="G16" s="4">
         <v>0.37207374340353461</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.21899708926559922</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" si="1"/>
+        <v>5.2659202041713926E-2</v>
+      </c>
+      <c r="J16" s="8">
+        <f t="shared" si="2"/>
+        <v>0.14152893875288078</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -902,8 +1127,20 @@
       <c r="G17" s="4">
         <v>0.52259977416900871</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="9">
+        <f t="shared" si="0"/>
+        <v>-9.3594946789519851E-2</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="1"/>
+        <v>0.10028423498104483</v>
+      </c>
+      <c r="J17" s="8">
+        <f t="shared" si="2"/>
+        <v>0.19189490684435873</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -925,8 +1162,20 @@
       <c r="G18" s="4">
         <v>42.131884429069459</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.24874671957401398</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" si="1"/>
+        <v>5.2809730060141291</v>
+      </c>
+      <c r="J18" s="8">
+        <f t="shared" si="2"/>
+        <v>0.12534385958702696</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -947,6 +1196,18 @@
       </c>
       <c r="G19" s="4">
         <v>879.62152969154806</v>
+      </c>
+      <c r="H19" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.25024622719728995</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>109.44624140304632</v>
+      </c>
+      <c r="J19" s="8">
+        <f t="shared" si="2"/>
+        <v>0.12442424123182298</v>
       </c>
     </row>
   </sheetData>
@@ -1416,15 +1677,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>25</v>
       </c>
@@ -1446,8 +1715,14 @@
       <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>26</v>
       </c>
@@ -1469,8 +1744,16 @@
       <c r="G2" s="7">
         <v>0.22487775651615191</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="9">
+        <f>(E2-G2)/G2</f>
+        <v>-0.12431720344705083</v>
+      </c>
+      <c r="I2" s="8">
+        <f>(C2-E2)/C2</f>
+        <v>0.25038494662063676</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>27</v>
       </c>
@@ -1492,8 +1775,16 @@
       <c r="G3" s="7">
         <v>6.9699873626627337E-5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="9">
+        <f t="shared" ref="H3:H4" si="0">(E3-G3)/G3</f>
+        <v>-0.1243293578489148</v>
+      </c>
+      <c r="I3" s="8">
+        <f t="shared" ref="I3:I4" si="1">(C3-E3)/C3</f>
+        <v>0.25049827176996781</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
@@ -1514,6 +1805,14 @@
       </c>
       <c r="G4" s="7">
         <v>0.128866444540544</v>
+      </c>
+      <c r="H4" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.16960758435337933</v>
+      </c>
+      <c r="I4" s="8">
+        <f t="shared" si="1"/>
+        <v>0.13498630368001469</v>
       </c>
     </row>
   </sheetData>
@@ -1525,16 +1824,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Scenario evaluation for Iris
</commit_message>
<xml_diff>
--- a/Outputs/Iris_mean_results.xlsx
+++ b/Outputs/Iris_mean_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giparoli\Documents\Projetos\AEco\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488DE89B-4270-43D4-AE50-CA6C0DC3772D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFB9573-6A17-48F3-BDBF-76EE970F806F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -133,9 +133,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +159,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,7 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -237,10 +243,12 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,7 +555,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1677,10 +1685,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1693,7 +1701,7 @@
     <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>25</v>
       </c>
@@ -1722,7 +1730,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>26</v>
       </c>
@@ -1752,8 +1760,15 @@
         <f>(C2-E2)/C2</f>
         <v>0.25038494662063676</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" s="11">
+        <v>0.19392999999999999</v>
+      </c>
+      <c r="K2" s="9">
+        <f>(J2-E2)/E2</f>
+        <v>-1.5191746214246699E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>27</v>
       </c>
@@ -1783,8 +1798,15 @@
         <f t="shared" ref="I3:I4" si="1">(C3-E3)/C3</f>
         <v>0.25049827176996781</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" s="11">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="K3" s="9">
+        <f t="shared" ref="K3:K4" si="2">(J3-E3)/E3</f>
+        <v>-1.6943520682821286E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
@@ -1814,9 +1836,23 @@
         <f t="shared" si="1"/>
         <v>0.13498630368001469</v>
       </c>
+      <c r="J4" s="11">
+        <v>0.10777299999999999</v>
+      </c>
+      <c r="K4" s="9">
+        <f t="shared" si="2"/>
+        <v>7.1328271411581446E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K5" s="12">
+        <f>AVERAGE(K2:K4)</f>
+        <v>-8.3341465853032804E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>